<commit_message>
updated sample data and SearchLine
</commit_message>
<xml_diff>
--- a/public/M1Database/index/Index_D.xlsx
+++ b/public/M1Database/index/Index_D.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jimmy\Desktop\Index\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\hardly-normal\public\M1Database\index\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{57DF3E12-AA21-419E-97CA-10CBD91A7E06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32E5D24F-BCC1-4544-92C0-C0494BFC2895}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6460" yWindow="11310" windowWidth="30930" windowHeight="15380" xr2:uid="{ECDF64F4-851C-4CAF-84F4-592D72488789}"/>
+    <workbookView xWindow="1100" yWindow="4120" windowWidth="24110" windowHeight="15380" xr2:uid="{ECDF64F4-851C-4CAF-84F4-592D72488789}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="8">
   <si>
     <t>LastName</t>
   </si>
@@ -415,7 +415,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -528,72 +528,20 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7">
-        <v>41000000022</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E7" s="2">
-        <v>43985</v>
-      </c>
+      <c r="D7" s="1"/>
+      <c r="E7" s="2"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8">
-        <v>41000000023</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E8" s="2">
-        <v>44350</v>
-      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="2"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9">
-        <v>41000000024</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E9" s="2">
-        <v>44715</v>
-      </c>
+      <c r="D9" s="1"/>
+      <c r="E9" s="2"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10">
-        <v>41000000025</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E10" s="2">
-        <v>45080</v>
-      </c>
+      <c r="D10" s="1"/>
+      <c r="E10" s="2"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D11" s="1"/>

</xml_diff>